<commit_message>
fixed error in week week two exercise
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{9644CC4E-8C7C-408A-B63D-E47D5EC83429}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{9A97CA6E-BA0F-4BC8-BE54-FBD1C3041C0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{15640CF8-077B-4002-A34F-D871E928D622}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="950" windowWidth="48840" windowHeight="21650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Codebook" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Height</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>Agecat</t>
+  </si>
+  <si>
+    <t>systolic_blood</t>
+  </si>
+  <si>
+    <t>Emp_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systolic Blood Pressure </t>
+  </si>
+  <si>
+    <t>Empl_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment Status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1= Full time employed, 2= part time, 3= unemployed </t>
   </si>
 </sst>
 </file>
@@ -404,15 +422,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,8 +449,14 @@
       <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>180</v>
       </c>
@@ -445,8 +472,16 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(90,200)</f>
+        <v>159</v>
+      </c>
+      <c r="G2">
+        <f ca="1">RANDBETWEEN(1,3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>175</v>
       </c>
@@ -462,8 +497,16 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <f t="shared" ref="F3:F15" ca="1" si="0">RANDBETWEEN(90,200)</f>
+        <v>117</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G15" ca="1" si="1">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -479,8 +522,16 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>178</v>
       </c>
@@ -496,8 +547,16 @@
       <c r="E5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>192</v>
       </c>
@@ -513,8 +572,16 @@
       <c r="E6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -530,8 +597,16 @@
       <c r="E7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>162</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>156</v>
       </c>
@@ -547,8 +622,16 @@
       <c r="E8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>166</v>
       </c>
@@ -564,8 +647,16 @@
       <c r="E9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>155</v>
       </c>
@@ -581,8 +672,16 @@
       <c r="E10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>162</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>145</v>
       </c>
@@ -598,8 +697,16 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>165</v>
       </c>
@@ -612,8 +719,16 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>133</v>
       </c>
@@ -629,8 +744,16 @@
       <c r="E13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>166</v>
       </c>
@@ -646,8 +769,16 @@
       <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>154</v>
       </c>
@@ -662,6 +793,14 @@
       </c>
       <c r="E15">
         <v>3</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -671,10 +810,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,8 +867,351 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="882513f6-57f1-402e-9cd4-ecb8f5f6b480" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062AF244E107AB5428D9DC167159A3393" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a9722de616b23fae40a3172095eccd93">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="882513f6-57f1-402e-9cd4-ecb8f5f6b480" xmlns:ns4="6cb85892-3e52-4f40-966a-40eea172498b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4c2b081c2517e0dc3dd18ae7ac6f8bf" ns1:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="882513f6-57f1-402e-9cd4-ecb8f5f6b480"/>
+    <xsd:import namespace="6cb85892-3e52-4f40-966a-40eea172498b"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="18" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="19" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="882513f6-57f1-402e-9cd4-ecb8f5f6b480" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_activity" ma:index="8" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="23" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="24" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="25" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6cb85892-3e52-4f40-966a-40eea172498b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="20" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="21" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="22" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB201122-1ABC-43D9-B136-E18D09470E37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6cb85892-3e52-4f40-966a-40eea172498b"/>
+    <ds:schemaRef ds:uri="882513f6-57f1-402e-9cd4-ecb8f5f6b480"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8249291-DDF7-4E5B-BC86-E2695DE3AF63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8749AAF4-84DE-440D-A8A8-C4DFF0E4FBED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="882513f6-57f1-402e-9cd4-ecb8f5f6b480"/>
+    <ds:schemaRef ds:uri="6cb85892-3e52-4f40-966a-40eea172498b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>